<commit_message>
MG-RAST results for sprague Jan2015 sample
results from running the Jan2015 FASTQ sample through
http://metagenomics.anl.gov/
</commit_message>
<xml_diff>
--- a/Data/sprague-ubiomeJan2015x.xlsx
+++ b/Data/sprague-ubiomeJan2015x.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sprague-ubiomeJan2015x.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="MGRAST" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MGRAST!$A$1:$B$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sprague-ubiomeJan2015x.csv'!$A$1:$H$525</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2104" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="549">
   <si>
     <t>parent</t>
   </si>
@@ -1654,16 +1656,47 @@
   </si>
   <si>
     <t>taxon</t>
+  </si>
+  <si>
+    <t>Arthropoda</t>
+  </si>
+  <si>
+    <t>Euryarchaeota</t>
+  </si>
+  <si>
+    <t>Streptophyta</t>
+  </si>
+  <si>
+    <t>unclassified (derived from Bacteria)</t>
+  </si>
+  <si>
+    <t>unclassified (derived from unclassified sequences)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1686,14 +1719,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2026,9 +2063,9 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H525"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="F528" sqref="F528:G540"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2089,7 +2126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1239</v>
       </c>
@@ -2245,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>976</v>
       </c>
@@ -2325,22 +2362,22 @@
     </row>
     <row r="12" spans="1:8" hidden="1">
       <c r="A12">
-        <v>31980</v>
+        <v>216851</v>
       </c>
       <c r="B12">
-        <v>186803</v>
+        <v>541000</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>16600</v>
       </c>
       <c r="D12">
-        <v>17</v>
+        <v>141979</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>508</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
@@ -2377,22 +2414,22 @@
     </row>
     <row r="14" spans="1:8" hidden="1">
       <c r="A14">
-        <v>904</v>
+        <v>816</v>
       </c>
       <c r="B14">
-        <v>909930</v>
+        <v>815</v>
       </c>
       <c r="C14">
-        <v>44</v>
+        <v>14869</v>
       </c>
       <c r="D14">
-        <v>376</v>
+        <v>127174</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>205</v>
+        <v>29</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
@@ -2401,7 +2438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15">
         <v>40520</v>
       </c>
@@ -2429,22 +2466,22 @@
     </row>
     <row r="16" spans="1:8" hidden="1">
       <c r="A16">
-        <v>447020</v>
+        <v>1263</v>
       </c>
       <c r="B16">
-        <v>84107</v>
+        <v>541000</v>
       </c>
       <c r="C16">
-        <v>19</v>
+        <v>9801</v>
       </c>
       <c r="D16">
-        <v>163</v>
+        <v>83827</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>246</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
@@ -2453,7 +2490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>201174</v>
       </c>
@@ -2557,7 +2594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21">
         <v>905</v>
       </c>
@@ -2637,22 +2674,22 @@
     </row>
     <row r="24" spans="1:8" hidden="1">
       <c r="A24">
-        <v>46352</v>
+        <v>1678</v>
       </c>
       <c r="B24">
-        <v>85023</v>
+        <v>31953</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>7777</v>
       </c>
       <c r="D24">
-        <v>17</v>
+        <v>66516</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>466</v>
+        <v>41</v>
       </c>
       <c r="G24" t="s">
         <v>27</v>
@@ -2663,22 +2700,22 @@
     </row>
     <row r="25" spans="1:8" hidden="1">
       <c r="A25">
-        <v>239934</v>
+        <v>1485</v>
       </c>
       <c r="B25">
-        <v>203557</v>
+        <v>31979</v>
       </c>
       <c r="C25">
-        <v>733</v>
+        <v>7730</v>
       </c>
       <c r="D25">
-        <v>6269</v>
+        <v>66114</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="G25" t="s">
         <v>27</v>
@@ -2689,22 +2726,22 @@
     </row>
     <row r="26" spans="1:8" hidden="1">
       <c r="A26">
-        <v>239759</v>
+        <v>33042</v>
       </c>
       <c r="B26">
-        <v>171550</v>
+        <v>186803</v>
       </c>
       <c r="C26">
-        <v>533</v>
+        <v>6326</v>
       </c>
       <c r="D26">
-        <v>4559</v>
+        <v>54106</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="G26" t="s">
         <v>27</v>
@@ -2713,7 +2750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" hidden="1">
       <c r="A27">
         <v>187327</v>
       </c>
@@ -2739,7 +2776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" hidden="1">
       <c r="A28">
         <v>446660</v>
       </c>
@@ -2767,22 +2804,22 @@
     </row>
     <row r="29" spans="1:8" hidden="1">
       <c r="A29">
-        <v>85924</v>
+        <v>572511</v>
       </c>
       <c r="B29">
-        <v>72276</v>
+        <v>186803</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>5225</v>
       </c>
       <c r="D29">
-        <v>60</v>
+        <v>44689</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>329</v>
+        <v>46</v>
       </c>
       <c r="G29" t="s">
         <v>27</v>
@@ -2793,22 +2830,22 @@
     </row>
     <row r="30" spans="1:8" hidden="1">
       <c r="A30">
-        <v>209879</v>
+        <v>841</v>
       </c>
       <c r="B30">
-        <v>31977</v>
+        <v>186803</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>5002</v>
       </c>
       <c r="D30">
-        <v>26</v>
+        <v>42782</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>419</v>
+        <v>47</v>
       </c>
       <c r="G30" t="s">
         <v>27</v>
@@ -2843,7 +2880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" hidden="1">
       <c r="A32">
         <v>214856</v>
       </c>
@@ -2869,7 +2906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" hidden="1">
       <c r="A33">
         <v>626932</v>
       </c>
@@ -2895,7 +2932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" hidden="1">
       <c r="A34">
         <v>328813</v>
       </c>
@@ -2947,7 +2984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" hidden="1">
       <c r="A36">
         <v>328814</v>
       </c>
@@ -2973,7 +3010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" hidden="1">
       <c r="A37">
         <v>938293</v>
       </c>
@@ -3051,7 +3088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" hidden="1">
       <c r="A40">
         <v>649756</v>
       </c>
@@ -3157,22 +3194,22 @@
     </row>
     <row r="44" spans="1:8" hidden="1">
       <c r="A44">
-        <v>165779</v>
+        <v>207244</v>
       </c>
       <c r="B44">
-        <v>543310</v>
+        <v>186803</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>2444</v>
       </c>
       <c r="D44">
-        <v>43</v>
+        <v>20903</v>
       </c>
       <c r="E44" t="s">
         <v>7</v>
       </c>
       <c r="F44" t="s">
-        <v>351</v>
+        <v>62</v>
       </c>
       <c r="G44" t="s">
         <v>27</v>
@@ -3183,22 +3220,22 @@
     </row>
     <row r="45" spans="1:8" hidden="1">
       <c r="A45">
-        <v>52784</v>
+        <v>46205</v>
       </c>
       <c r="B45">
-        <v>541000</v>
+        <v>186803</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2109</v>
       </c>
       <c r="D45">
-        <v>26</v>
+        <v>18038</v>
       </c>
       <c r="E45" t="s">
         <v>7</v>
       </c>
       <c r="F45" t="s">
-        <v>398</v>
+        <v>63</v>
       </c>
       <c r="G45" t="s">
         <v>27</v>
@@ -3207,7 +3244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" hidden="1">
       <c r="A46">
         <v>169435</v>
       </c>
@@ -3233,7 +3270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" hidden="1">
       <c r="A47">
         <v>545498</v>
       </c>
@@ -3313,22 +3350,22 @@
     </row>
     <row r="50" spans="1:8" hidden="1">
       <c r="A50">
-        <v>264995</v>
+        <v>283168</v>
       </c>
       <c r="B50">
-        <v>186806</v>
+        <v>171551</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>1295</v>
       </c>
       <c r="D50">
-        <v>26</v>
+        <v>11076</v>
       </c>
       <c r="E50" t="s">
         <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>415</v>
+        <v>68</v>
       </c>
       <c r="G50" t="s">
         <v>27</v>
@@ -3337,7 +3374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>1224</v>
       </c>
@@ -3365,22 +3402,22 @@
     </row>
     <row r="52" spans="1:8" hidden="1">
       <c r="A52">
-        <v>653683</v>
+        <v>28050</v>
       </c>
       <c r="B52">
-        <v>31979</v>
+        <v>186803</v>
       </c>
       <c r="C52">
-        <v>41</v>
+        <v>1143</v>
       </c>
       <c r="D52">
-        <v>351</v>
+        <v>9776</v>
       </c>
       <c r="E52" t="s">
         <v>7</v>
       </c>
       <c r="F52" t="s">
-        <v>212</v>
+        <v>71</v>
       </c>
       <c r="G52" t="s">
         <v>27</v>
@@ -3389,7 +3426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" hidden="1">
       <c r="A53">
         <v>98671</v>
       </c>
@@ -3415,7 +3452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" hidden="1">
       <c r="A54">
         <v>1390</v>
       </c>
@@ -3441,7 +3478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" hidden="1">
       <c r="A55">
         <v>653685</v>
       </c>
@@ -3495,22 +3532,22 @@
     </row>
     <row r="57" spans="1:8" hidden="1">
       <c r="A57">
-        <v>207244</v>
+        <v>189330</v>
       </c>
       <c r="B57">
         <v>186803</v>
       </c>
       <c r="C57">
-        <v>2444</v>
+        <v>870</v>
       </c>
       <c r="D57">
-        <v>20903</v>
+        <v>7441</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
       </c>
       <c r="F57" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="G57" t="s">
         <v>27</v>
@@ -3545,7 +3582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>74201</v>
       </c>
@@ -3651,22 +3688,22 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63">
-        <v>244127</v>
+        <v>239934</v>
       </c>
       <c r="B63">
-        <v>541000</v>
+        <v>203557</v>
       </c>
       <c r="C63">
-        <v>60</v>
+        <v>733</v>
       </c>
       <c r="D63">
-        <v>513</v>
+        <v>6269</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
       </c>
       <c r="F63" t="s">
-        <v>188</v>
+        <v>83</v>
       </c>
       <c r="G63" t="s">
         <v>27</v>
@@ -3675,7 +3712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" hidden="1">
       <c r="A64">
         <v>157956</v>
       </c>
@@ -3755,22 +3792,22 @@
     </row>
     <row r="67" spans="1:8" hidden="1">
       <c r="A67">
-        <v>1663</v>
+        <v>1716</v>
       </c>
       <c r="B67">
-        <v>1268</v>
+        <v>1653</v>
       </c>
       <c r="C67">
-        <v>147</v>
+        <v>657</v>
       </c>
       <c r="D67">
-        <v>1257</v>
+        <v>5619</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
       </c>
       <c r="F67" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="G67" t="s">
         <v>27</v>
@@ -3857,7 +3894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" hidden="1">
       <c r="A71">
         <v>1201401</v>
       </c>
@@ -3911,22 +3948,22 @@
     </row>
     <row r="73" spans="1:8" hidden="1">
       <c r="A73">
-        <v>1386</v>
+        <v>375288</v>
       </c>
       <c r="B73">
-        <v>186817</v>
+        <v>171551</v>
       </c>
       <c r="C73">
-        <v>85</v>
+        <v>593</v>
       </c>
       <c r="D73">
-        <v>727</v>
+        <v>5072</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>
       </c>
       <c r="F73" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
       <c r="G73" t="s">
         <v>27</v>
@@ -3937,22 +3974,22 @@
     </row>
     <row r="74" spans="1:8" hidden="1">
       <c r="A74">
-        <v>816</v>
+        <v>397864</v>
       </c>
       <c r="B74">
-        <v>815</v>
+        <v>171551</v>
       </c>
       <c r="C74">
-        <v>14869</v>
+        <v>545</v>
       </c>
       <c r="D74">
-        <v>127174</v>
+        <v>4661</v>
       </c>
       <c r="E74" t="s">
         <v>7</v>
       </c>
       <c r="F74" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="G74" t="s">
         <v>27</v>
@@ -3961,7 +3998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" hidden="1">
       <c r="A75">
         <v>1201878</v>
       </c>
@@ -3987,7 +4024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" hidden="1">
       <c r="A76">
         <v>1146058</v>
       </c>
@@ -4015,22 +4052,22 @@
     </row>
     <row r="77" spans="1:8" hidden="1">
       <c r="A77">
-        <v>397864</v>
+        <v>239759</v>
       </c>
       <c r="B77">
-        <v>171551</v>
+        <v>171550</v>
       </c>
       <c r="C77">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="D77">
-        <v>4661</v>
+        <v>4559</v>
       </c>
       <c r="E77" t="s">
         <v>7</v>
       </c>
       <c r="F77" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G77" t="s">
         <v>27</v>
@@ -4039,7 +4076,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" hidden="1">
       <c r="A78">
         <v>1146296</v>
       </c>
@@ -4065,7 +4102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" hidden="1">
       <c r="A79">
         <v>1146723</v>
       </c>
@@ -4197,22 +4234,22 @@
     </row>
     <row r="84" spans="1:8" hidden="1">
       <c r="A84">
-        <v>1678</v>
+        <v>577310</v>
       </c>
       <c r="B84">
-        <v>31953</v>
+        <v>995019</v>
       </c>
       <c r="C84">
-        <v>7777</v>
+        <v>449</v>
       </c>
       <c r="D84">
-        <v>66516</v>
+        <v>3840</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="G84" t="s">
         <v>27</v>
@@ -4221,7 +4258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" hidden="1">
       <c r="A85">
         <v>1118061</v>
       </c>
@@ -4249,22 +4286,22 @@
     </row>
     <row r="86" spans="1:8" hidden="1">
       <c r="A86">
-        <v>35832</v>
+        <v>1266</v>
       </c>
       <c r="B86">
-        <v>194924</v>
+        <v>31979</v>
       </c>
       <c r="C86">
-        <v>74</v>
+        <v>387</v>
       </c>
       <c r="D86">
-        <v>633</v>
+        <v>3310</v>
       </c>
       <c r="E86" t="s">
         <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="G86" t="s">
         <v>27</v>
@@ -4301,22 +4338,22 @@
     </row>
     <row r="88" spans="1:8" hidden="1">
       <c r="A88">
-        <v>572511</v>
+        <v>39948</v>
       </c>
       <c r="B88">
-        <v>186803</v>
+        <v>31977</v>
       </c>
       <c r="C88">
-        <v>5225</v>
+        <v>373</v>
       </c>
       <c r="D88">
-        <v>44689</v>
+        <v>3190</v>
       </c>
       <c r="E88" t="s">
         <v>7</v>
       </c>
       <c r="F88" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="G88" t="s">
         <v>27</v>
@@ -4353,22 +4390,22 @@
     </row>
     <row r="90" spans="1:8" hidden="1">
       <c r="A90">
-        <v>29521</v>
+        <v>1730</v>
       </c>
       <c r="B90">
-        <v>143786</v>
+        <v>186806</v>
       </c>
       <c r="C90">
-        <v>10</v>
+        <v>348</v>
       </c>
       <c r="D90">
-        <v>86</v>
+        <v>2976</v>
       </c>
       <c r="E90" t="s">
         <v>7</v>
       </c>
       <c r="F90" t="s">
-        <v>286</v>
+        <v>111</v>
       </c>
       <c r="G90" t="s">
         <v>27</v>
@@ -4377,7 +4414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" hidden="1">
       <c r="A91">
         <v>47678</v>
       </c>
@@ -4431,22 +4468,22 @@
     </row>
     <row r="93" spans="1:8" hidden="1">
       <c r="A93">
-        <v>1696</v>
+        <v>1301</v>
       </c>
       <c r="B93">
-        <v>85019</v>
+        <v>1300</v>
       </c>
       <c r="C93">
-        <v>24</v>
+        <v>307</v>
       </c>
       <c r="D93">
-        <v>205</v>
+        <v>2626</v>
       </c>
       <c r="E93" t="s">
         <v>7</v>
       </c>
       <c r="F93" t="s">
-        <v>235</v>
+        <v>114</v>
       </c>
       <c r="G93" t="s">
         <v>27</v>
@@ -4455,7 +4492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" hidden="1">
       <c r="A94">
         <v>290053</v>
       </c>
@@ -4481,7 +4518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" hidden="1">
       <c r="A95">
         <v>329854</v>
       </c>
@@ -4507,7 +4544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" hidden="1">
       <c r="A96">
         <v>204516</v>
       </c>
@@ -4559,7 +4596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" hidden="1">
       <c r="A98">
         <v>28116</v>
       </c>
@@ -4611,7 +4648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" hidden="1">
       <c r="A100">
         <v>310297</v>
       </c>
@@ -4663,7 +4700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" hidden="1">
       <c r="A102">
         <v>691816</v>
       </c>
@@ -4715,7 +4752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" hidden="1">
       <c r="A104">
         <v>291644</v>
       </c>
@@ -4741,7 +4778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" hidden="1">
       <c r="A105">
         <v>820</v>
       </c>
@@ -4795,22 +4832,22 @@
     </row>
     <row r="107" spans="1:8" hidden="1">
       <c r="A107">
-        <v>41275</v>
+        <v>830</v>
       </c>
       <c r="B107">
-        <v>76892</v>
+        <v>186803</v>
       </c>
       <c r="C107">
-        <v>53</v>
+        <v>199</v>
       </c>
       <c r="D107">
-        <v>453</v>
+        <v>1702</v>
       </c>
       <c r="E107" t="s">
         <v>7</v>
       </c>
       <c r="F107" t="s">
-        <v>193</v>
+        <v>128</v>
       </c>
       <c r="G107" t="s">
         <v>27</v>
@@ -4819,7 +4856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" hidden="1">
       <c r="A108">
         <v>821</v>
       </c>
@@ -4873,22 +4910,22 @@
     </row>
     <row r="110" spans="1:8" hidden="1">
       <c r="A110">
-        <v>574697</v>
+        <v>1578</v>
       </c>
       <c r="B110">
-        <v>171551</v>
+        <v>33958</v>
       </c>
       <c r="C110">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D110">
-        <v>1394</v>
+        <v>1437</v>
       </c>
       <c r="E110" t="s">
         <v>7</v>
       </c>
       <c r="F110" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G110" t="s">
         <v>27</v>
@@ -4897,7 +4934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" hidden="1">
       <c r="A111">
         <v>487174</v>
       </c>
@@ -4925,22 +4962,22 @@
     </row>
     <row r="112" spans="1:8" hidden="1">
       <c r="A112">
-        <v>830</v>
+        <v>574697</v>
       </c>
       <c r="B112">
-        <v>186803</v>
+        <v>171551</v>
       </c>
       <c r="C112">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="D112">
-        <v>1702</v>
+        <v>1394</v>
       </c>
       <c r="E112" t="s">
         <v>7</v>
       </c>
       <c r="F112" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="G112" t="s">
         <v>27</v>
@@ -5003,22 +5040,22 @@
     </row>
     <row r="115" spans="1:8" hidden="1">
       <c r="A115">
-        <v>249529</v>
+        <v>1663</v>
       </c>
       <c r="B115">
-        <v>186814</v>
+        <v>1268</v>
       </c>
       <c r="C115">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="D115">
-        <v>17</v>
+        <v>1257</v>
       </c>
       <c r="E115" t="s">
         <v>7</v>
       </c>
       <c r="F115" t="s">
-        <v>540</v>
+        <v>136</v>
       </c>
       <c r="G115" t="s">
         <v>27</v>
@@ -5053,7 +5090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" hidden="1">
       <c r="A117">
         <v>1680</v>
       </c>
@@ -5079,7 +5116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" hidden="1">
       <c r="A118">
         <v>28025</v>
       </c>
@@ -5313,7 +5350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1">
+    <row r="127" spans="1:8">
       <c r="A127">
         <v>508458</v>
       </c>
@@ -5471,22 +5508,22 @@
     </row>
     <row r="133" spans="1:8" hidden="1">
       <c r="A133">
-        <v>44258</v>
+        <v>292632</v>
       </c>
       <c r="B133">
-        <v>31979</v>
+        <v>541000</v>
       </c>
       <c r="C133">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="D133">
-        <v>488</v>
+        <v>992</v>
       </c>
       <c r="E133" t="s">
         <v>7</v>
       </c>
       <c r="F133" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="G133" t="s">
         <v>27</v>
@@ -5497,22 +5534,22 @@
     </row>
     <row r="134" spans="1:8" hidden="1">
       <c r="A134">
-        <v>698776</v>
+        <v>191303</v>
       </c>
       <c r="B134">
-        <v>186803</v>
+        <v>128827</v>
       </c>
       <c r="C134">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="D134">
-        <v>205</v>
+        <v>881</v>
       </c>
       <c r="E134" t="s">
         <v>7</v>
       </c>
       <c r="F134" t="s">
-        <v>236</v>
+        <v>156</v>
       </c>
       <c r="G134" t="s">
         <v>27</v>
@@ -5599,7 +5636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" hidden="1">
       <c r="A138">
         <v>1681</v>
       </c>
@@ -5653,22 +5690,22 @@
     </row>
     <row r="140" spans="1:8" hidden="1">
       <c r="A140">
-        <v>990721</v>
+        <v>596767</v>
       </c>
       <c r="B140">
-        <v>990719</v>
+        <v>541000</v>
       </c>
       <c r="C140">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="D140">
-        <v>17</v>
+        <v>787</v>
       </c>
       <c r="E140" t="s">
         <v>7</v>
       </c>
       <c r="F140" t="s">
-        <v>484</v>
+        <v>162</v>
       </c>
       <c r="G140" t="s">
         <v>27</v>
@@ -5677,7 +5714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" hidden="1">
       <c r="A141">
         <v>1685</v>
       </c>
@@ -5705,22 +5742,22 @@
     </row>
     <row r="142" spans="1:8" hidden="1">
       <c r="A142">
-        <v>1485</v>
+        <v>1386</v>
       </c>
       <c r="B142">
-        <v>31979</v>
+        <v>186817</v>
       </c>
       <c r="C142">
-        <v>7730</v>
+        <v>85</v>
       </c>
       <c r="D142">
-        <v>66114</v>
+        <v>727</v>
       </c>
       <c r="E142" t="s">
         <v>7</v>
       </c>
       <c r="F142" t="s">
-        <v>42</v>
+        <v>164</v>
       </c>
       <c r="G142" t="s">
         <v>27</v>
@@ -5757,22 +5794,22 @@
     </row>
     <row r="144" spans="1:8" hidden="1">
       <c r="A144">
-        <v>102106</v>
+        <v>638847</v>
       </c>
       <c r="B144">
-        <v>84107</v>
+        <v>649777</v>
       </c>
       <c r="C144">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="D144">
-        <v>163</v>
+        <v>727</v>
       </c>
       <c r="E144" t="s">
         <v>7</v>
       </c>
       <c r="F144" t="s">
-        <v>248</v>
+        <v>166</v>
       </c>
       <c r="G144" t="s">
         <v>27</v>
@@ -5781,7 +5818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" hidden="1">
       <c r="A145">
         <v>216816</v>
       </c>
@@ -5807,7 +5844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" hidden="1">
       <c r="A146">
         <v>78346</v>
       </c>
@@ -5859,7 +5896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1">
+    <row r="148" spans="1:8">
       <c r="A148">
         <v>544448</v>
       </c>
@@ -5887,22 +5924,22 @@
     </row>
     <row r="149" spans="1:8" hidden="1">
       <c r="A149">
-        <v>33042</v>
+        <v>35832</v>
       </c>
       <c r="B149">
-        <v>186803</v>
+        <v>194924</v>
       </c>
       <c r="C149">
-        <v>6326</v>
+        <v>74</v>
       </c>
       <c r="D149">
-        <v>54106</v>
+        <v>633</v>
       </c>
       <c r="E149" t="s">
         <v>7</v>
       </c>
       <c r="F149" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="G149" t="s">
         <v>27</v>
@@ -5911,7 +5948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" hidden="1">
       <c r="A150">
         <v>78257</v>
       </c>
@@ -5989,7 +6026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" hidden="1">
       <c r="A153">
         <v>35833</v>
       </c>
@@ -6015,7 +6052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" hidden="1">
       <c r="A154">
         <v>871665</v>
       </c>
@@ -6041,7 +6078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" hidden="1">
       <c r="A155">
         <v>871664</v>
       </c>
@@ -6147,22 +6184,22 @@
     </row>
     <row r="159" spans="1:8" hidden="1">
       <c r="A159">
-        <v>1716</v>
+        <v>963</v>
       </c>
       <c r="B159">
-        <v>1653</v>
+        <v>75682</v>
       </c>
       <c r="C159">
-        <v>657</v>
+        <v>64</v>
       </c>
       <c r="D159">
-        <v>5619</v>
+        <v>547</v>
       </c>
       <c r="E159" t="s">
         <v>7</v>
       </c>
       <c r="F159" t="s">
-        <v>88</v>
+        <v>182</v>
       </c>
       <c r="G159" t="s">
         <v>27</v>
@@ -6173,22 +6210,22 @@
     </row>
     <row r="160" spans="1:8" hidden="1">
       <c r="A160">
-        <v>413496</v>
+        <v>1472762</v>
       </c>
       <c r="B160">
-        <v>543</v>
+        <v>84107</v>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="D160">
-        <v>17</v>
+        <v>530</v>
       </c>
       <c r="E160" t="s">
         <v>7</v>
       </c>
       <c r="F160" t="s">
-        <v>490</v>
+        <v>183</v>
       </c>
       <c r="G160" t="s">
         <v>27</v>
@@ -6223,7 +6260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" hidden="1">
       <c r="A162">
         <v>1203227</v>
       </c>
@@ -6303,22 +6340,22 @@
     </row>
     <row r="165" spans="1:8" hidden="1">
       <c r="A165">
-        <v>167375</v>
+        <v>244127</v>
       </c>
       <c r="B165">
-        <v>1118</v>
+        <v>541000</v>
       </c>
       <c r="C165">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="D165">
-        <v>17</v>
+        <v>513</v>
       </c>
       <c r="E165" t="s">
         <v>7</v>
       </c>
       <c r="F165" t="s">
-        <v>527</v>
+        <v>188</v>
       </c>
       <c r="G165" t="s">
         <v>27</v>
@@ -6327,7 +6364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" hidden="1">
       <c r="A166">
         <v>576927</v>
       </c>
@@ -6355,22 +6392,22 @@
     </row>
     <row r="167" spans="1:8" hidden="1">
       <c r="A167">
-        <v>79603</v>
+        <v>44258</v>
       </c>
       <c r="B167">
-        <v>84107</v>
+        <v>31979</v>
       </c>
       <c r="C167">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="D167">
-        <v>34</v>
+        <v>488</v>
       </c>
       <c r="E167" t="s">
         <v>7</v>
       </c>
       <c r="F167" t="s">
-        <v>380</v>
+        <v>190</v>
       </c>
       <c r="G167" t="s">
         <v>27</v>
@@ -6381,22 +6418,22 @@
     </row>
     <row r="168" spans="1:8" hidden="1">
       <c r="A168">
-        <v>36853</v>
+        <v>248744</v>
       </c>
       <c r="B168">
-        <v>186807</v>
+        <v>186803</v>
       </c>
       <c r="C168">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D168">
-        <v>17</v>
+        <v>479</v>
       </c>
       <c r="E168" t="s">
         <v>7</v>
       </c>
       <c r="F168" t="s">
-        <v>532</v>
+        <v>191</v>
       </c>
       <c r="G168" t="s">
         <v>27</v>
@@ -6433,22 +6470,22 @@
     </row>
     <row r="170" spans="1:8" hidden="1">
       <c r="A170">
-        <v>89342</v>
+        <v>41275</v>
       </c>
       <c r="B170">
-        <v>213119</v>
+        <v>76892</v>
       </c>
       <c r="C170">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D170">
-        <v>17</v>
+        <v>453</v>
       </c>
       <c r="E170" t="s">
         <v>7</v>
       </c>
       <c r="F170" t="s">
-        <v>436</v>
+        <v>193</v>
       </c>
       <c r="G170" t="s">
         <v>27</v>
@@ -6457,7 +6494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" hidden="1">
       <c r="A171">
         <v>53363</v>
       </c>
@@ -6509,7 +6546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" hidden="1">
       <c r="A173">
         <v>105829</v>
       </c>
@@ -6665,7 +6702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1">
+    <row r="179" spans="1:8">
       <c r="A179">
         <v>57723</v>
       </c>
@@ -6693,22 +6730,22 @@
     </row>
     <row r="180" spans="1:8" hidden="1">
       <c r="A180">
-        <v>79206</v>
+        <v>33024</v>
       </c>
       <c r="B180">
-        <v>186807</v>
+        <v>909930</v>
       </c>
       <c r="C180">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="D180">
-        <v>26</v>
+        <v>393</v>
       </c>
       <c r="E180" t="s">
         <v>7</v>
       </c>
       <c r="F180" t="s">
-        <v>429</v>
+        <v>203</v>
       </c>
       <c r="G180" t="s">
         <v>27</v>
@@ -6745,22 +6782,22 @@
     </row>
     <row r="182" spans="1:8" hidden="1">
       <c r="A182">
-        <v>872</v>
+        <v>904</v>
       </c>
       <c r="B182">
-        <v>194924</v>
+        <v>909930</v>
       </c>
       <c r="C182">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D182">
-        <v>137</v>
+        <v>376</v>
       </c>
       <c r="E182" t="s">
         <v>7</v>
       </c>
       <c r="F182" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
       <c r="G182" t="s">
         <v>27</v>
@@ -6771,22 +6808,22 @@
     </row>
     <row r="183" spans="1:8" hidden="1">
       <c r="A183">
-        <v>427925</v>
+        <v>255204</v>
       </c>
       <c r="B183">
-        <v>68298</v>
+        <v>85023</v>
       </c>
       <c r="C183">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="D183">
-        <v>17</v>
+        <v>376</v>
       </c>
       <c r="E183" t="s">
         <v>7</v>
       </c>
       <c r="F183" t="s">
-        <v>455</v>
+        <v>206</v>
       </c>
       <c r="G183" t="s">
         <v>27</v>
@@ -6795,7 +6832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" hidden="1">
       <c r="A184">
         <v>340474</v>
       </c>
@@ -6821,7 +6858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" hidden="1">
       <c r="A185">
         <v>1217281</v>
       </c>
@@ -6847,7 +6884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" hidden="1">
       <c r="A186">
         <v>544645</v>
       </c>
@@ -6873,7 +6910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" hidden="1">
       <c r="A187">
         <v>911092</v>
       </c>
@@ -6899,7 +6936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" hidden="1">
       <c r="A188">
         <v>537373</v>
       </c>
@@ -6927,22 +6964,22 @@
     </row>
     <row r="189" spans="1:8" hidden="1">
       <c r="A189">
-        <v>39948</v>
+        <v>653683</v>
       </c>
       <c r="B189">
-        <v>31977</v>
+        <v>31979</v>
       </c>
       <c r="C189">
-        <v>373</v>
+        <v>41</v>
       </c>
       <c r="D189">
-        <v>3190</v>
+        <v>351</v>
       </c>
       <c r="E189" t="s">
         <v>7</v>
       </c>
       <c r="F189" t="s">
-        <v>109</v>
+        <v>212</v>
       </c>
       <c r="G189" t="s">
         <v>27</v>
@@ -6951,7 +6988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" hidden="1">
       <c r="A190">
         <v>620860</v>
       </c>
@@ -6979,22 +7016,22 @@
     </row>
     <row r="191" spans="1:8" hidden="1">
       <c r="A191">
-        <v>189330</v>
+        <v>838</v>
       </c>
       <c r="B191">
-        <v>186803</v>
+        <v>171552</v>
       </c>
       <c r="C191">
-        <v>870</v>
+        <v>39</v>
       </c>
       <c r="D191">
-        <v>7441</v>
+        <v>334</v>
       </c>
       <c r="E191" t="s">
         <v>7</v>
       </c>
       <c r="F191" t="s">
-        <v>76</v>
+        <v>214</v>
       </c>
       <c r="G191" t="s">
         <v>27</v>
@@ -7029,7 +7066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" hidden="1">
       <c r="A193">
         <v>189710</v>
       </c>
@@ -7081,7 +7118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" hidden="1">
       <c r="A195">
         <v>1561</v>
       </c>
@@ -7109,22 +7146,22 @@
     </row>
     <row r="196" spans="1:8" hidden="1">
       <c r="A196">
-        <v>156973</v>
+        <v>168934</v>
       </c>
       <c r="B196">
-        <v>171551</v>
+        <v>41295</v>
       </c>
       <c r="C196">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D196">
-        <v>120</v>
+        <v>299</v>
       </c>
       <c r="E196" t="s">
         <v>7</v>
       </c>
       <c r="F196" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
       <c r="G196" t="s">
         <v>27</v>
@@ -7135,22 +7172,22 @@
     </row>
     <row r="197" spans="1:8" hidden="1">
       <c r="A197">
-        <v>1472762</v>
+        <v>150022</v>
       </c>
       <c r="B197">
-        <v>84107</v>
+        <v>543310</v>
       </c>
       <c r="C197">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="D197">
-        <v>530</v>
+        <v>291</v>
       </c>
       <c r="E197" t="s">
         <v>7</v>
       </c>
       <c r="F197" t="s">
-        <v>183</v>
+        <v>220</v>
       </c>
       <c r="G197" t="s">
         <v>27</v>
@@ -7159,7 +7196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" hidden="1">
       <c r="A198">
         <v>1491</v>
       </c>
@@ -7185,7 +7222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" hidden="1">
       <c r="A199">
         <v>29356</v>
       </c>
@@ -7213,22 +7250,22 @@
     </row>
     <row r="200" spans="1:8" hidden="1">
       <c r="A200">
-        <v>2383</v>
+        <v>2753</v>
       </c>
       <c r="B200">
-        <v>186813</v>
+        <v>649777</v>
       </c>
       <c r="C200">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D200">
-        <v>17</v>
+        <v>274</v>
       </c>
       <c r="E200" t="s">
         <v>7</v>
       </c>
       <c r="F200" t="s">
-        <v>477</v>
+        <v>223</v>
       </c>
       <c r="G200" t="s">
         <v>27</v>
@@ -7237,7 +7274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" hidden="1">
       <c r="A201">
         <v>46867</v>
       </c>
@@ -7263,7 +7300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" hidden="1">
       <c r="A202">
         <v>288965</v>
       </c>
@@ -7289,7 +7326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" hidden="1">
       <c r="A203">
         <v>1531</v>
       </c>
@@ -7315,7 +7352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" hidden="1">
       <c r="A204">
         <v>84024</v>
       </c>
@@ -7341,7 +7378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" hidden="1">
       <c r="A205">
         <v>69825</v>
       </c>
@@ -7393,7 +7430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" hidden="1">
       <c r="A207">
         <v>84030</v>
       </c>
@@ -7419,7 +7456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" hidden="1">
       <c r="A208">
         <v>1217283</v>
       </c>
@@ -7473,22 +7510,22 @@
     </row>
     <row r="210" spans="1:8" hidden="1">
       <c r="A210">
-        <v>1730</v>
+        <v>2701</v>
       </c>
       <c r="B210">
-        <v>186806</v>
+        <v>31953</v>
       </c>
       <c r="C210">
-        <v>348</v>
+        <v>25</v>
       </c>
       <c r="D210">
-        <v>2976</v>
+        <v>214</v>
       </c>
       <c r="E210" t="s">
         <v>7</v>
       </c>
       <c r="F210" t="s">
-        <v>111</v>
+        <v>233</v>
       </c>
       <c r="G210" t="s">
         <v>27</v>
@@ -7525,22 +7562,22 @@
     </row>
     <row r="212" spans="1:8" hidden="1">
       <c r="A212">
-        <v>216851</v>
+        <v>1696</v>
       </c>
       <c r="B212">
-        <v>541000</v>
+        <v>85019</v>
       </c>
       <c r="C212">
-        <v>16600</v>
+        <v>24</v>
       </c>
       <c r="D212">
-        <v>141979</v>
+        <v>205</v>
       </c>
       <c r="E212" t="s">
         <v>7</v>
       </c>
       <c r="F212" t="s">
-        <v>26</v>
+        <v>235</v>
       </c>
       <c r="G212" t="s">
         <v>27</v>
@@ -7551,22 +7588,22 @@
     </row>
     <row r="213" spans="1:8" hidden="1">
       <c r="A213">
-        <v>150022</v>
+        <v>698776</v>
       </c>
       <c r="B213">
-        <v>543310</v>
+        <v>186803</v>
       </c>
       <c r="C213">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D213">
-        <v>291</v>
+        <v>205</v>
       </c>
       <c r="E213" t="s">
         <v>7</v>
       </c>
       <c r="F213" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="G213" t="s">
         <v>27</v>
@@ -7575,7 +7612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" hidden="1">
       <c r="A214">
         <v>691811</v>
       </c>
@@ -7601,7 +7638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" hidden="1">
       <c r="A215">
         <v>320882</v>
       </c>
@@ -7731,7 +7768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" hidden="1">
       <c r="A220">
         <v>227526</v>
       </c>
@@ -7757,7 +7794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="221" spans="1:8" hidden="1">
+    <row r="221" spans="1:8">
       <c r="A221">
         <v>256845</v>
       </c>
@@ -7811,22 +7848,22 @@
     </row>
     <row r="223" spans="1:8" hidden="1">
       <c r="A223">
-        <v>946234</v>
+        <v>447020</v>
       </c>
       <c r="B223">
-        <v>186813</v>
+        <v>84107</v>
       </c>
       <c r="C223">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D223">
-        <v>17</v>
+        <v>163</v>
       </c>
       <c r="E223" t="s">
         <v>7</v>
       </c>
       <c r="F223" t="s">
-        <v>457</v>
+        <v>246</v>
       </c>
       <c r="G223" t="s">
         <v>27</v>
@@ -7835,7 +7872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" hidden="1">
       <c r="A224">
         <v>545497</v>
       </c>
@@ -7863,22 +7900,22 @@
     </row>
     <row r="225" spans="1:8" hidden="1">
       <c r="A225">
-        <v>311207</v>
+        <v>102106</v>
       </c>
       <c r="B225">
-        <v>49546</v>
+        <v>84107</v>
       </c>
       <c r="C225">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D225">
-        <v>34</v>
+        <v>163</v>
       </c>
       <c r="E225" t="s">
         <v>7</v>
       </c>
       <c r="F225" t="s">
-        <v>360</v>
+        <v>248</v>
       </c>
       <c r="G225" t="s">
         <v>27</v>
@@ -7887,7 +7924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1">
+    <row r="226" spans="1:8">
       <c r="A226">
         <v>65842</v>
       </c>
@@ -7939,7 +7976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" hidden="1">
       <c r="A228">
         <v>626944</v>
       </c>
@@ -7967,22 +8004,22 @@
     </row>
     <row r="229" spans="1:8" hidden="1">
       <c r="A229">
-        <v>2701</v>
+        <v>90243</v>
       </c>
       <c r="B229">
-        <v>31953</v>
+        <v>506</v>
       </c>
       <c r="C229">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D229">
-        <v>214</v>
+        <v>145</v>
       </c>
       <c r="E229" t="s">
         <v>7</v>
       </c>
       <c r="F229" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="G229" t="s">
         <v>27</v>
@@ -7993,22 +8030,22 @@
     </row>
     <row r="230" spans="1:8" hidden="1">
       <c r="A230">
-        <v>644652</v>
+        <v>40544</v>
       </c>
       <c r="B230">
-        <v>84107</v>
+        <v>995019</v>
       </c>
       <c r="C230">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D230">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="E230" t="s">
         <v>7</v>
       </c>
       <c r="F230" t="s">
-        <v>315</v>
+        <v>253</v>
       </c>
       <c r="G230" t="s">
         <v>27</v>
@@ -8069,7 +8106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" hidden="1">
       <c r="A233">
         <v>1512</v>
       </c>
@@ -8149,22 +8186,22 @@
     </row>
     <row r="236" spans="1:8" hidden="1">
       <c r="A236">
-        <v>471824</v>
+        <v>872</v>
       </c>
       <c r="B236">
-        <v>471823</v>
+        <v>194924</v>
       </c>
       <c r="C236">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D236">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="E236" t="s">
         <v>7</v>
       </c>
       <c r="F236" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="G236" t="s">
         <v>27</v>
@@ -8173,7 +8210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" hidden="1">
       <c r="A237">
         <v>1232426</v>
       </c>
@@ -8277,7 +8314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" hidden="1">
       <c r="A241">
         <v>116085</v>
       </c>
@@ -8329,7 +8366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" hidden="1">
       <c r="A243">
         <v>410072</v>
       </c>
@@ -8383,22 +8420,22 @@
     </row>
     <row r="245" spans="1:8" hidden="1">
       <c r="A245">
-        <v>209</v>
+        <v>156973</v>
       </c>
       <c r="B245">
-        <v>72293</v>
+        <v>171551</v>
       </c>
       <c r="C245">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D245">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="E245" t="s">
         <v>7</v>
       </c>
       <c r="F245" t="s">
-        <v>533</v>
+        <v>267</v>
       </c>
       <c r="G245" t="s">
         <v>27</v>
@@ -8487,22 +8524,22 @@
     </row>
     <row r="249" spans="1:8" hidden="1">
       <c r="A249">
-        <v>963</v>
+        <v>459786</v>
       </c>
       <c r="B249">
-        <v>75682</v>
+        <v>216572</v>
       </c>
       <c r="C249">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D249">
-        <v>547</v>
+        <v>111</v>
       </c>
       <c r="E249" t="s">
         <v>7</v>
       </c>
       <c r="F249" t="s">
-        <v>182</v>
+        <v>273</v>
       </c>
       <c r="G249" t="s">
         <v>27</v>
@@ -8511,7 +8548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" hidden="1">
       <c r="A250">
         <v>537278</v>
       </c>
@@ -8539,22 +8576,22 @@
     </row>
     <row r="251" spans="1:8" hidden="1">
       <c r="A251">
-        <v>596767</v>
+        <v>44249</v>
       </c>
       <c r="B251">
-        <v>541000</v>
+        <v>186822</v>
       </c>
       <c r="C251">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="D251">
-        <v>787</v>
+        <v>111</v>
       </c>
       <c r="E251" t="s">
         <v>7</v>
       </c>
       <c r="F251" t="s">
-        <v>162</v>
+        <v>271</v>
       </c>
       <c r="G251" t="s">
         <v>27</v>
@@ -8563,7 +8600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" hidden="1">
       <c r="A252">
         <v>1232436</v>
       </c>
@@ -8589,7 +8626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" hidden="1">
       <c r="A253">
         <v>38284</v>
       </c>
@@ -8669,22 +8706,22 @@
     </row>
     <row r="256" spans="1:8" hidden="1">
       <c r="A256">
-        <v>57493</v>
+        <v>471824</v>
       </c>
       <c r="B256">
-        <v>1268</v>
+        <v>471823</v>
       </c>
       <c r="C256">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D256">
-        <v>17</v>
+        <v>103</v>
       </c>
       <c r="E256" t="s">
         <v>7</v>
       </c>
       <c r="F256" t="s">
-        <v>538</v>
+        <v>278</v>
       </c>
       <c r="G256" t="s">
         <v>27</v>
@@ -8745,7 +8782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" hidden="1">
       <c r="A259">
         <v>43765</v>
       </c>
@@ -8773,22 +8810,22 @@
     </row>
     <row r="260" spans="1:8" hidden="1">
       <c r="A260">
-        <v>28050</v>
+        <v>437755</v>
       </c>
       <c r="B260">
         <v>186803</v>
       </c>
       <c r="C260">
-        <v>1143</v>
+        <v>11</v>
       </c>
       <c r="D260">
-        <v>9776</v>
+        <v>94</v>
       </c>
       <c r="E260" t="s">
         <v>7</v>
       </c>
       <c r="F260" t="s">
-        <v>71</v>
+        <v>284</v>
       </c>
       <c r="G260" t="s">
         <v>27</v>
@@ -8825,22 +8862,22 @@
     </row>
     <row r="262" spans="1:8" hidden="1">
       <c r="A262">
-        <v>1578</v>
+        <v>196082</v>
       </c>
       <c r="B262">
-        <v>33958</v>
+        <v>31953</v>
       </c>
       <c r="C262">
-        <v>168</v>
+        <v>11</v>
       </c>
       <c r="D262">
-        <v>1437</v>
+        <v>94</v>
       </c>
       <c r="E262" t="s">
         <v>7</v>
       </c>
       <c r="F262" t="s">
-        <v>131</v>
+        <v>282</v>
       </c>
       <c r="G262" t="s">
         <v>27</v>
@@ -8877,22 +8914,22 @@
     </row>
     <row r="264" spans="1:8" hidden="1">
       <c r="A264">
-        <v>445</v>
+        <v>29521</v>
       </c>
       <c r="B264">
-        <v>444</v>
+        <v>143786</v>
       </c>
       <c r="C264">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D264">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="E264" t="s">
         <v>7</v>
       </c>
       <c r="F264" t="s">
-        <v>476</v>
+        <v>286</v>
       </c>
       <c r="G264" t="s">
         <v>27</v>
@@ -8901,7 +8938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" hidden="1">
       <c r="A265">
         <v>134034</v>
       </c>
@@ -8979,7 +9016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="268" spans="1:8" hidden="1">
+    <row r="268" spans="1:8">
       <c r="A268">
         <v>203691</v>
       </c>
@@ -9083,7 +9120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" hidden="1">
       <c r="A272">
         <v>38288</v>
       </c>
@@ -9111,22 +9148,22 @@
     </row>
     <row r="273" spans="1:8" hidden="1">
       <c r="A273">
-        <v>1637</v>
+        <v>354349</v>
       </c>
       <c r="B273">
-        <v>186820</v>
+        <v>118882</v>
       </c>
       <c r="C273">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D273">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="E273" t="s">
         <v>7</v>
       </c>
       <c r="F273" t="s">
-        <v>405</v>
+        <v>295</v>
       </c>
       <c r="G273" t="s">
         <v>27</v>
@@ -9161,7 +9198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" hidden="1">
       <c r="A275">
         <v>38289</v>
       </c>
@@ -9265,7 +9302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="279" spans="1:8" hidden="1">
+    <row r="279" spans="1:8">
       <c r="A279">
         <v>200795</v>
       </c>
@@ -9291,7 +9328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" hidden="1">
       <c r="A280">
         <v>57171</v>
       </c>
@@ -9317,7 +9354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" hidden="1">
       <c r="A281">
         <v>1719</v>
       </c>
@@ -9343,7 +9380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" hidden="1">
       <c r="A282">
         <v>702953</v>
       </c>
@@ -9525,7 +9562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
+    <row r="289" spans="1:8" hidden="1">
       <c r="A289">
         <v>28141</v>
       </c>
@@ -9551,7 +9588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="290" spans="1:8">
+    <row r="290" spans="1:8" hidden="1">
       <c r="A290">
         <v>142877</v>
       </c>
@@ -9605,22 +9642,22 @@
     </row>
     <row r="292" spans="1:8" hidden="1">
       <c r="A292">
-        <v>85076</v>
+        <v>184869</v>
       </c>
       <c r="B292">
-        <v>1046</v>
+        <v>2049</v>
       </c>
       <c r="C292">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D292">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="E292" t="s">
         <v>7</v>
       </c>
       <c r="F292" t="s">
-        <v>483</v>
+        <v>313</v>
       </c>
       <c r="G292" t="s">
         <v>27</v>
@@ -9657,22 +9694,22 @@
     </row>
     <row r="294" spans="1:8" hidden="1">
       <c r="A294">
-        <v>248744</v>
+        <v>644652</v>
       </c>
       <c r="B294">
-        <v>186803</v>
+        <v>84107</v>
       </c>
       <c r="C294">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D294">
-        <v>479</v>
+        <v>68</v>
       </c>
       <c r="E294" t="s">
         <v>7</v>
       </c>
       <c r="F294" t="s">
-        <v>191</v>
+        <v>315</v>
       </c>
       <c r="G294" t="s">
         <v>27</v>
@@ -9681,7 +9718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="295" spans="1:8" hidden="1">
+    <row r="295" spans="1:8">
       <c r="A295">
         <v>1134404</v>
       </c>
@@ -9735,22 +9772,22 @@
     </row>
     <row r="297" spans="1:8" hidden="1">
       <c r="A297">
-        <v>1295378</v>
+        <v>1427376</v>
       </c>
       <c r="B297">
-        <v>403</v>
+        <v>84107</v>
       </c>
       <c r="C297">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D297">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="E297" t="s">
         <v>7</v>
       </c>
       <c r="F297" t="s">
-        <v>467</v>
+        <v>318</v>
       </c>
       <c r="G297" t="s">
         <v>27</v>
@@ -9811,7 +9848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="300" spans="1:8" hidden="1">
+    <row r="300" spans="1:8">
       <c r="A300">
         <v>67819</v>
       </c>
@@ -9837,7 +9874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="301" spans="1:8">
+    <row r="301" spans="1:8" hidden="1">
       <c r="A301">
         <v>79209</v>
       </c>
@@ -9863,7 +9900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="302" spans="1:8">
+    <row r="302" spans="1:8" hidden="1">
       <c r="A302">
         <v>134223</v>
       </c>
@@ -9889,7 +9926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="303" spans="1:8" hidden="1">
+    <row r="303" spans="1:8">
       <c r="A303">
         <v>40117</v>
       </c>
@@ -9967,7 +10004,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="306" spans="1:8">
+    <row r="306" spans="1:8" hidden="1">
       <c r="A306">
         <v>427926</v>
       </c>
@@ -10021,22 +10058,22 @@
     </row>
     <row r="308" spans="1:8" hidden="1">
       <c r="A308">
-        <v>437755</v>
+        <v>85924</v>
       </c>
       <c r="B308">
-        <v>186803</v>
+        <v>72276</v>
       </c>
       <c r="C308">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D308">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="E308" t="s">
         <v>7</v>
       </c>
       <c r="F308" t="s">
-        <v>284</v>
+        <v>329</v>
       </c>
       <c r="G308" t="s">
         <v>27</v>
@@ -10071,7 +10108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="310" spans="1:8">
+    <row r="310" spans="1:8" hidden="1">
       <c r="A310">
         <v>39486</v>
       </c>
@@ -10151,22 +10188,22 @@
     </row>
     <row r="313" spans="1:8" hidden="1">
       <c r="A313">
-        <v>1161127</v>
+        <v>2740</v>
       </c>
       <c r="B313">
-        <v>186804</v>
+        <v>186807</v>
       </c>
       <c r="C313">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D313">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E313" t="s">
         <v>7</v>
       </c>
       <c r="F313" t="s">
-        <v>388</v>
+        <v>334</v>
       </c>
       <c r="G313" t="s">
         <v>27</v>
@@ -10175,7 +10212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="314" spans="1:8" hidden="1">
+    <row r="314" spans="1:8">
       <c r="A314">
         <v>1117</v>
       </c>
@@ -10253,7 +10290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="317" spans="1:8">
+    <row r="317" spans="1:8" hidden="1">
       <c r="A317">
         <v>1472761</v>
       </c>
@@ -10331,7 +10368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:8" hidden="1">
       <c r="A320">
         <v>39484</v>
       </c>
@@ -10385,22 +10422,22 @@
     </row>
     <row r="322" spans="1:8" hidden="1">
       <c r="A322">
-        <v>354354</v>
+        <v>162289</v>
       </c>
       <c r="B322">
-        <v>563835</v>
+        <v>543310</v>
       </c>
       <c r="C322">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D322">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="E322" t="s">
         <v>7</v>
       </c>
       <c r="F322" t="s">
-        <v>481</v>
+        <v>343</v>
       </c>
       <c r="G322" t="s">
         <v>27</v>
@@ -10513,7 +10550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="327" spans="1:8">
+    <row r="327" spans="1:8" hidden="1">
       <c r="A327">
         <v>39485</v>
       </c>
@@ -10565,7 +10602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="329" spans="1:8">
+    <row r="329" spans="1:8" hidden="1">
       <c r="A329">
         <v>39488</v>
       </c>
@@ -10593,22 +10630,22 @@
     </row>
     <row r="330" spans="1:8" hidden="1">
       <c r="A330">
-        <v>283168</v>
+        <v>165779</v>
       </c>
       <c r="B330">
-        <v>171551</v>
+        <v>543310</v>
       </c>
       <c r="C330">
-        <v>1295</v>
+        <v>5</v>
       </c>
       <c r="D330">
-        <v>11076</v>
+        <v>43</v>
       </c>
       <c r="E330" t="s">
         <v>7</v>
       </c>
       <c r="F330" t="s">
-        <v>68</v>
+        <v>351</v>
       </c>
       <c r="G330" t="s">
         <v>27</v>
@@ -10617,7 +10654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="331" spans="1:8">
+    <row r="331" spans="1:8" hidden="1">
       <c r="A331">
         <v>39492</v>
       </c>
@@ -10669,7 +10706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="333" spans="1:8">
+    <row r="333" spans="1:8" hidden="1">
       <c r="A333">
         <v>39497</v>
       </c>
@@ -10721,7 +10758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="335" spans="1:8">
+    <row r="335" spans="1:8" hidden="1">
       <c r="A335">
         <v>853</v>
       </c>
@@ -10827,22 +10864,22 @@
     </row>
     <row r="339" spans="1:8" hidden="1">
       <c r="A339">
-        <v>90243</v>
+        <v>79603</v>
       </c>
       <c r="B339">
-        <v>506</v>
+        <v>84107</v>
       </c>
       <c r="C339">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D339">
-        <v>145</v>
+        <v>34</v>
       </c>
       <c r="E339" t="s">
         <v>7</v>
       </c>
       <c r="F339" t="s">
-        <v>252</v>
+        <v>380</v>
       </c>
       <c r="G339" t="s">
         <v>27</v>
@@ -10853,22 +10890,22 @@
     </row>
     <row r="340" spans="1:8" hidden="1">
       <c r="A340">
-        <v>265975</v>
+        <v>311207</v>
       </c>
       <c r="B340">
-        <v>186803</v>
+        <v>49546</v>
       </c>
       <c r="C340">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D340">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E340" t="s">
         <v>7</v>
       </c>
       <c r="F340" t="s">
-        <v>529</v>
+        <v>360</v>
       </c>
       <c r="G340" t="s">
         <v>27</v>
@@ -11215,7 +11252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="354" spans="1:8">
+    <row r="354" spans="1:8" hidden="1">
       <c r="A354">
         <v>1260</v>
       </c>
@@ -11267,7 +11304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="356" spans="1:8">
+    <row r="356" spans="1:8" hidden="1">
       <c r="A356">
         <v>292800</v>
       </c>
@@ -11347,22 +11384,22 @@
     </row>
     <row r="359" spans="1:8" hidden="1">
       <c r="A359">
-        <v>459786</v>
+        <v>1161127</v>
       </c>
       <c r="B359">
-        <v>216572</v>
+        <v>186804</v>
       </c>
       <c r="C359">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D359">
-        <v>111</v>
+        <v>34</v>
       </c>
       <c r="E359" t="s">
         <v>7</v>
       </c>
       <c r="F359" t="s">
-        <v>273</v>
+        <v>388</v>
       </c>
       <c r="G359" t="s">
         <v>27</v>
@@ -11475,7 +11512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="364" spans="1:8">
+    <row r="364" spans="1:8" hidden="1">
       <c r="A364">
         <v>471189</v>
       </c>
@@ -11527,7 +11564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="366" spans="1:8">
+    <row r="366" spans="1:8" hidden="1">
       <c r="A366">
         <v>471825</v>
       </c>
@@ -11555,22 +11592,22 @@
     </row>
     <row r="367" spans="1:8" hidden="1">
       <c r="A367">
-        <v>44249</v>
+        <v>1017280</v>
       </c>
       <c r="B367">
-        <v>186822</v>
+        <v>186813</v>
       </c>
       <c r="C367">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D367">
-        <v>111</v>
+        <v>34</v>
       </c>
       <c r="E367" t="s">
         <v>7</v>
       </c>
       <c r="F367" t="s">
-        <v>271</v>
+        <v>361</v>
       </c>
       <c r="G367" t="s">
         <v>27</v>
@@ -11605,7 +11642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="369" spans="1:8">
+    <row r="369" spans="1:8" hidden="1">
       <c r="A369">
         <v>631628</v>
       </c>
@@ -11735,7 +11772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="374" spans="1:8">
+    <row r="374" spans="1:8" hidden="1">
       <c r="A374">
         <v>658081</v>
       </c>
@@ -11761,7 +11798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="375" spans="1:8">
+    <row r="375" spans="1:8" hidden="1">
       <c r="A375">
         <v>706562</v>
       </c>
@@ -11787,7 +11824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="376" spans="1:8">
+    <row r="376" spans="1:8" hidden="1">
       <c r="A376">
         <v>1295382</v>
       </c>
@@ -11815,22 +11852,22 @@
     </row>
     <row r="377" spans="1:8" hidden="1">
       <c r="A377">
-        <v>100175</v>
+        <v>209879</v>
       </c>
       <c r="B377">
-        <v>541000</v>
+        <v>31977</v>
       </c>
       <c r="C377">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D377">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E377" t="s">
         <v>7</v>
       </c>
       <c r="F377" t="s">
-        <v>470</v>
+        <v>419</v>
       </c>
       <c r="G377" t="s">
         <v>27</v>
@@ -11841,22 +11878,22 @@
     </row>
     <row r="378" spans="1:8" hidden="1">
       <c r="A378">
-        <v>375288</v>
+        <v>52784</v>
       </c>
       <c r="B378">
-        <v>171551</v>
+        <v>541000</v>
       </c>
       <c r="C378">
-        <v>593</v>
+        <v>3</v>
       </c>
       <c r="D378">
-        <v>5072</v>
+        <v>26</v>
       </c>
       <c r="E378" t="s">
         <v>7</v>
       </c>
       <c r="F378" t="s">
-        <v>94</v>
+        <v>398</v>
       </c>
       <c r="G378" t="s">
         <v>27</v>
@@ -11917,7 +11954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="381" spans="1:8">
+    <row r="381" spans="1:8" hidden="1">
       <c r="A381">
         <v>626933</v>
       </c>
@@ -11943,7 +11980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="382" spans="1:8">
+    <row r="382" spans="1:8" hidden="1">
       <c r="A382">
         <v>28118</v>
       </c>
@@ -11969,7 +12006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="383" spans="1:8">
+    <row r="383" spans="1:8" hidden="1">
       <c r="A383">
         <v>90245</v>
       </c>
@@ -12049,22 +12086,22 @@
     </row>
     <row r="386" spans="1:8" hidden="1">
       <c r="A386">
-        <v>196082</v>
+        <v>264995</v>
       </c>
       <c r="B386">
-        <v>31953</v>
+        <v>186806</v>
       </c>
       <c r="C386">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D386">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="E386" t="s">
         <v>7</v>
       </c>
       <c r="F386" t="s">
-        <v>282</v>
+        <v>415</v>
       </c>
       <c r="G386" t="s">
         <v>27</v>
@@ -12127,22 +12164,22 @@
     </row>
     <row r="389" spans="1:8" hidden="1">
       <c r="A389">
-        <v>577310</v>
+        <v>79206</v>
       </c>
       <c r="B389">
-        <v>995019</v>
+        <v>186807</v>
       </c>
       <c r="C389">
-        <v>449</v>
+        <v>3</v>
       </c>
       <c r="D389">
-        <v>3840</v>
+        <v>26</v>
       </c>
       <c r="E389" t="s">
         <v>7</v>
       </c>
       <c r="F389" t="s">
-        <v>105</v>
+        <v>429</v>
       </c>
       <c r="G389" t="s">
         <v>27</v>
@@ -12229,7 +12266,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="393" spans="1:8">
+    <row r="393" spans="1:8" hidden="1">
       <c r="A393">
         <v>823</v>
       </c>
@@ -12255,7 +12292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="394" spans="1:8" hidden="1">
+    <row r="394" spans="1:8">
       <c r="A394">
         <v>1090</v>
       </c>
@@ -12309,22 +12346,22 @@
     </row>
     <row r="396" spans="1:8" hidden="1">
       <c r="A396">
-        <v>1427376</v>
+        <v>1637</v>
       </c>
       <c r="B396">
-        <v>84107</v>
+        <v>186820</v>
       </c>
       <c r="C396">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D396">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="E396" t="s">
         <v>7</v>
       </c>
       <c r="F396" t="s">
-        <v>318</v>
+        <v>405</v>
       </c>
       <c r="G396" t="s">
         <v>27</v>
@@ -12359,7 +12396,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="398" spans="1:8">
+    <row r="398" spans="1:8" hidden="1">
       <c r="A398">
         <v>387661</v>
       </c>
@@ -12413,22 +12450,22 @@
     </row>
     <row r="400" spans="1:8" hidden="1">
       <c r="A400">
-        <v>84567</v>
+        <v>323449</v>
       </c>
       <c r="B400">
-        <v>84566</v>
+        <v>89373</v>
       </c>
       <c r="C400">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D400">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E400" t="s">
         <v>7</v>
       </c>
       <c r="F400" t="s">
-        <v>537</v>
+        <v>397</v>
       </c>
       <c r="G400" t="s">
         <v>27</v>
@@ -12439,22 +12476,22 @@
     </row>
     <row r="401" spans="1:8" hidden="1">
       <c r="A401">
-        <v>2740</v>
+        <v>40840</v>
       </c>
       <c r="B401">
-        <v>186807</v>
+        <v>909930</v>
       </c>
       <c r="C401">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D401">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="E401" t="s">
         <v>7</v>
       </c>
       <c r="F401" t="s">
-        <v>334</v>
+        <v>408</v>
       </c>
       <c r="G401" t="s">
         <v>27</v>
@@ -12463,7 +12500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="402" spans="1:8">
+    <row r="402" spans="1:8" hidden="1">
       <c r="A402">
         <v>46503</v>
       </c>
@@ -12489,7 +12526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="403" spans="1:8">
+    <row r="403" spans="1:8" hidden="1">
       <c r="A403">
         <v>487175</v>
       </c>
@@ -12515,7 +12552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="404" spans="1:8">
+    <row r="404" spans="1:8" hidden="1">
       <c r="A404">
         <v>747645</v>
       </c>
@@ -12619,7 +12656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="408" spans="1:8">
+    <row r="408" spans="1:8" hidden="1">
       <c r="A408">
         <v>2741</v>
       </c>
@@ -12645,7 +12682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="409" spans="1:8">
+    <row r="409" spans="1:8" hidden="1">
       <c r="A409">
         <v>411567</v>
       </c>
@@ -12673,22 +12710,22 @@
     </row>
     <row r="410" spans="1:8" hidden="1">
       <c r="A410">
-        <v>162289</v>
+        <v>278993</v>
       </c>
       <c r="B410">
-        <v>543310</v>
+        <v>186807</v>
       </c>
       <c r="C410">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D410">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="E410" t="s">
         <v>7</v>
       </c>
       <c r="F410" t="s">
-        <v>343</v>
+        <v>420</v>
       </c>
       <c r="G410" t="s">
         <v>27</v>
@@ -12853,7 +12890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="417" spans="1:8">
+    <row r="417" spans="1:8" hidden="1">
       <c r="A417">
         <v>33030</v>
       </c>
@@ -12881,22 +12918,22 @@
     </row>
     <row r="418" spans="1:8" hidden="1">
       <c r="A418">
-        <v>33024</v>
+        <v>31980</v>
       </c>
       <c r="B418">
-        <v>909930</v>
+        <v>186803</v>
       </c>
       <c r="C418">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="D418">
-        <v>393</v>
+        <v>17</v>
       </c>
       <c r="E418" t="s">
         <v>7</v>
       </c>
       <c r="F418" t="s">
-        <v>203</v>
+        <v>508</v>
       </c>
       <c r="G418" t="s">
         <v>27</v>
@@ -12907,22 +12944,22 @@
     </row>
     <row r="419" spans="1:8" hidden="1">
       <c r="A419">
-        <v>323449</v>
+        <v>46352</v>
       </c>
       <c r="B419">
-        <v>89373</v>
+        <v>85023</v>
       </c>
       <c r="C419">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D419">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E419" t="s">
         <v>7</v>
       </c>
       <c r="F419" t="s">
-        <v>397</v>
+        <v>466</v>
       </c>
       <c r="G419" t="s">
         <v>27</v>
@@ -12957,7 +12994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="421" spans="1:8">
+    <row r="421" spans="1:8" hidden="1">
       <c r="A421">
         <v>747603</v>
       </c>
@@ -12983,7 +13020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="422" spans="1:8">
+    <row r="422" spans="1:8" hidden="1">
       <c r="A422">
         <v>33025</v>
       </c>
@@ -13037,10 +13074,10 @@
     </row>
     <row r="424" spans="1:8" hidden="1">
       <c r="A424">
-        <v>836</v>
+        <v>249529</v>
       </c>
       <c r="B424">
-        <v>171551</v>
+        <v>186814</v>
       </c>
       <c r="C424">
         <v>2</v>
@@ -13052,7 +13089,7 @@
         <v>7</v>
       </c>
       <c r="F424" t="s">
-        <v>442</v>
+        <v>540</v>
       </c>
       <c r="G424" t="s">
         <v>27</v>
@@ -13113,7 +13150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="427" spans="1:8">
+    <row r="427" spans="1:8" hidden="1">
       <c r="A427">
         <v>1229957</v>
       </c>
@@ -13139,7 +13176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="428" spans="1:8">
+    <row r="428" spans="1:8" hidden="1">
       <c r="A428">
         <v>501496</v>
       </c>
@@ -13165,7 +13202,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="429" spans="1:8">
+    <row r="429" spans="1:8" hidden="1">
       <c r="A429">
         <v>28127</v>
       </c>
@@ -13243,7 +13280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="432" spans="1:8">
+    <row r="432" spans="1:8" hidden="1">
       <c r="A432">
         <v>641484</v>
       </c>
@@ -13373,7 +13410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="437" spans="1:8" hidden="1">
+    <row r="437" spans="1:8">
       <c r="A437">
         <v>200930</v>
       </c>
@@ -13401,22 +13438,22 @@
     </row>
     <row r="438" spans="1:8" hidden="1">
       <c r="A438">
-        <v>838</v>
+        <v>990721</v>
       </c>
       <c r="B438">
-        <v>171552</v>
+        <v>990719</v>
       </c>
       <c r="C438">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D438">
-        <v>334</v>
+        <v>17</v>
       </c>
       <c r="E438" t="s">
         <v>7</v>
       </c>
       <c r="F438" t="s">
-        <v>214</v>
+        <v>484</v>
       </c>
       <c r="G438" t="s">
         <v>27</v>
@@ -13425,7 +13462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="439" spans="1:8">
+    <row r="439" spans="1:8" hidden="1">
       <c r="A439">
         <v>106588</v>
       </c>
@@ -13453,22 +13490,22 @@
     </row>
     <row r="440" spans="1:8" hidden="1">
       <c r="A440">
-        <v>46205</v>
+        <v>413496</v>
       </c>
       <c r="B440">
-        <v>186803</v>
+        <v>543</v>
       </c>
       <c r="C440">
-        <v>2109</v>
+        <v>2</v>
       </c>
       <c r="D440">
-        <v>18038</v>
+        <v>17</v>
       </c>
       <c r="E440" t="s">
         <v>7</v>
       </c>
       <c r="F440" t="s">
-        <v>63</v>
+        <v>490</v>
       </c>
       <c r="G440" t="s">
         <v>27</v>
@@ -13477,7 +13514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="441" spans="1:8">
+    <row r="441" spans="1:8" hidden="1">
       <c r="A441">
         <v>360807</v>
       </c>
@@ -13687,22 +13724,22 @@
     </row>
     <row r="449" spans="1:8" hidden="1">
       <c r="A449">
-        <v>354349</v>
+        <v>167375</v>
       </c>
       <c r="B449">
-        <v>118882</v>
+        <v>1118</v>
       </c>
       <c r="C449">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D449">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="E449" t="s">
         <v>7</v>
       </c>
       <c r="F449" t="s">
-        <v>295</v>
+        <v>527</v>
       </c>
       <c r="G449" t="s">
         <v>27</v>
@@ -13713,22 +13750,22 @@
     </row>
     <row r="450" spans="1:8" hidden="1">
       <c r="A450">
-        <v>255204</v>
+        <v>36853</v>
       </c>
       <c r="B450">
-        <v>85023</v>
+        <v>186807</v>
       </c>
       <c r="C450">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="D450">
-        <v>376</v>
+        <v>17</v>
       </c>
       <c r="E450" t="s">
         <v>7</v>
       </c>
       <c r="F450" t="s">
-        <v>206</v>
+        <v>532</v>
       </c>
       <c r="G450" t="s">
         <v>27</v>
@@ -13763,7 +13800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="452" spans="1:8">
+    <row r="452" spans="1:8" hidden="1">
       <c r="A452">
         <v>583272</v>
       </c>
@@ -13791,22 +13828,22 @@
     </row>
     <row r="453" spans="1:8" hidden="1">
       <c r="A453">
-        <v>1017280</v>
+        <v>89342</v>
       </c>
       <c r="B453">
-        <v>186813</v>
+        <v>213119</v>
       </c>
       <c r="C453">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D453">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E453" t="s">
         <v>7</v>
       </c>
       <c r="F453" t="s">
-        <v>361</v>
+        <v>436</v>
       </c>
       <c r="G453" t="s">
         <v>27</v>
@@ -13841,7 +13878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="455" spans="1:8">
+    <row r="455" spans="1:8" hidden="1">
       <c r="A455">
         <v>877428</v>
       </c>
@@ -13867,7 +13904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="456" spans="1:8">
+    <row r="456" spans="1:8" hidden="1">
       <c r="A456">
         <v>40518</v>
       </c>
@@ -13947,22 +13984,22 @@
     </row>
     <row r="459" spans="1:8" hidden="1">
       <c r="A459">
-        <v>638847</v>
+        <v>427925</v>
       </c>
       <c r="B459">
-        <v>649777</v>
+        <v>68298</v>
       </c>
       <c r="C459">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="D459">
-        <v>727</v>
+        <v>17</v>
       </c>
       <c r="E459" t="s">
         <v>7</v>
       </c>
       <c r="F459" t="s">
-        <v>166</v>
+        <v>455</v>
       </c>
       <c r="G459" t="s">
         <v>27</v>
@@ -13973,22 +14010,22 @@
     </row>
     <row r="460" spans="1:8" hidden="1">
       <c r="A460">
-        <v>841</v>
+        <v>2383</v>
       </c>
       <c r="B460">
-        <v>186803</v>
+        <v>186813</v>
       </c>
       <c r="C460">
-        <v>5002</v>
+        <v>2</v>
       </c>
       <c r="D460">
-        <v>42782</v>
+        <v>17</v>
       </c>
       <c r="E460" t="s">
         <v>7</v>
       </c>
       <c r="F460" t="s">
-        <v>47</v>
+        <v>477</v>
       </c>
       <c r="G460" t="s">
         <v>27</v>
@@ -14051,22 +14088,22 @@
     </row>
     <row r="463" spans="1:8" hidden="1">
       <c r="A463">
-        <v>1263</v>
+        <v>946234</v>
       </c>
       <c r="B463">
-        <v>541000</v>
+        <v>186813</v>
       </c>
       <c r="C463">
-        <v>9801</v>
+        <v>2</v>
       </c>
       <c r="D463">
-        <v>83827</v>
+        <v>17</v>
       </c>
       <c r="E463" t="s">
         <v>7</v>
       </c>
       <c r="F463" t="s">
-        <v>32</v>
+        <v>457</v>
       </c>
       <c r="G463" t="s">
         <v>27</v>
@@ -14077,22 +14114,22 @@
     </row>
     <row r="464" spans="1:8" hidden="1">
       <c r="A464">
-        <v>1266</v>
+        <v>209</v>
       </c>
       <c r="B464">
-        <v>31979</v>
+        <v>72293</v>
       </c>
       <c r="C464">
-        <v>387</v>
+        <v>2</v>
       </c>
       <c r="D464">
-        <v>3310</v>
+        <v>17</v>
       </c>
       <c r="E464" t="s">
         <v>7</v>
       </c>
       <c r="F464" t="s">
-        <v>107</v>
+        <v>533</v>
       </c>
       <c r="G464" t="s">
         <v>27</v>
@@ -14101,7 +14138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="465" spans="1:8">
+    <row r="465" spans="1:8" hidden="1">
       <c r="A465">
         <v>592978</v>
       </c>
@@ -14129,10 +14166,10 @@
     </row>
     <row r="466" spans="1:8" hidden="1">
       <c r="A466">
-        <v>100132</v>
+        <v>57493</v>
       </c>
       <c r="B466">
-        <v>186803</v>
+        <v>1268</v>
       </c>
       <c r="C466">
         <v>2</v>
@@ -14144,7 +14181,7 @@
         <v>7</v>
       </c>
       <c r="F466" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
       <c r="G466" t="s">
         <v>27</v>
@@ -14155,10 +14192,10 @@
     </row>
     <row r="467" spans="1:8" hidden="1">
       <c r="A467">
-        <v>1279</v>
+        <v>445</v>
       </c>
       <c r="B467">
-        <v>90964</v>
+        <v>444</v>
       </c>
       <c r="C467">
         <v>2</v>
@@ -14170,7 +14207,7 @@
         <v>7</v>
       </c>
       <c r="F467" t="s">
-        <v>437</v>
+        <v>476</v>
       </c>
       <c r="G467" t="s">
         <v>27</v>
@@ -14179,7 +14216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="468" spans="1:8" hidden="1">
+    <row r="468" spans="1:8">
       <c r="A468">
         <v>142182</v>
       </c>
@@ -14205,7 +14242,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="469" spans="1:8">
+    <row r="469" spans="1:8" hidden="1">
       <c r="A469">
         <v>1265</v>
       </c>
@@ -14231,7 +14268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="470" spans="1:8">
+    <row r="470" spans="1:8" hidden="1">
       <c r="A470">
         <v>46228</v>
       </c>
@@ -14283,7 +14320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="472" spans="1:8">
+    <row r="472" spans="1:8" hidden="1">
       <c r="A472">
         <v>169434</v>
       </c>
@@ -14311,22 +14348,22 @@
     </row>
     <row r="473" spans="1:8" hidden="1">
       <c r="A473">
-        <v>1301</v>
+        <v>85076</v>
       </c>
       <c r="B473">
-        <v>1300</v>
+        <v>1046</v>
       </c>
       <c r="C473">
-        <v>307</v>
+        <v>2</v>
       </c>
       <c r="D473">
-        <v>2626</v>
+        <v>17</v>
       </c>
       <c r="E473" t="s">
         <v>7</v>
       </c>
       <c r="F473" t="s">
-        <v>114</v>
+        <v>483</v>
       </c>
       <c r="G473" t="s">
         <v>27</v>
@@ -14439,7 +14476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="478" spans="1:8">
+    <row r="478" spans="1:8" hidden="1">
       <c r="A478">
         <v>1101723</v>
       </c>
@@ -14517,7 +14554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="481" spans="1:8">
+    <row r="481" spans="1:8" hidden="1">
       <c r="A481">
         <v>361101</v>
       </c>
@@ -14595,7 +14632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="484" spans="1:8">
+    <row r="484" spans="1:8" hidden="1">
       <c r="A484">
         <v>1234680</v>
       </c>
@@ -14699,7 +14736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="488" spans="1:8">
+    <row r="488" spans="1:8" hidden="1">
       <c r="A488">
         <v>310942</v>
       </c>
@@ -14751,7 +14788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="490" spans="1:8">
+    <row r="490" spans="1:8" hidden="1">
       <c r="A490">
         <v>1308</v>
       </c>
@@ -14779,22 +14816,22 @@
     </row>
     <row r="491" spans="1:8" hidden="1">
       <c r="A491">
-        <v>292632</v>
+        <v>1295378</v>
       </c>
       <c r="B491">
-        <v>541000</v>
+        <v>403</v>
       </c>
       <c r="C491">
-        <v>116</v>
+        <v>2</v>
       </c>
       <c r="D491">
-        <v>992</v>
+        <v>17</v>
       </c>
       <c r="E491" t="s">
         <v>7</v>
       </c>
       <c r="F491" t="s">
-        <v>155</v>
+        <v>467</v>
       </c>
       <c r="G491" t="s">
         <v>27</v>
@@ -14803,7 +14840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="492" spans="1:8">
+    <row r="492" spans="1:8" hidden="1">
       <c r="A492">
         <v>665956</v>
       </c>
@@ -15011,7 +15048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="500" spans="1:8">
+    <row r="500" spans="1:8" hidden="1">
       <c r="A500">
         <v>214851</v>
       </c>
@@ -15037,7 +15074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="501" spans="1:8">
+    <row r="501" spans="1:8" hidden="1">
       <c r="A501">
         <v>457415</v>
       </c>
@@ -15141,7 +15178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="505" spans="1:8">
+    <row r="505" spans="1:8" hidden="1">
       <c r="A505">
         <v>863643</v>
       </c>
@@ -15193,7 +15230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="507" spans="1:8">
+    <row r="507" spans="1:8" hidden="1">
       <c r="A507">
         <v>154288</v>
       </c>
@@ -15273,22 +15310,22 @@
     </row>
     <row r="510" spans="1:8" hidden="1">
       <c r="A510">
-        <v>40840</v>
+        <v>354354</v>
       </c>
       <c r="B510">
-        <v>909930</v>
+        <v>563835</v>
       </c>
       <c r="C510">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D510">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E510" t="s">
         <v>7</v>
       </c>
       <c r="F510" t="s">
-        <v>408</v>
+        <v>481</v>
       </c>
       <c r="G510" t="s">
         <v>27</v>
@@ -15299,22 +15336,22 @@
     </row>
     <row r="511" spans="1:8" hidden="1">
       <c r="A511">
-        <v>40544</v>
+        <v>265975</v>
       </c>
       <c r="B511">
-        <v>995019</v>
+        <v>186803</v>
       </c>
       <c r="C511">
+        <v>2</v>
+      </c>
+      <c r="D511">
         <v>17</v>
       </c>
-      <c r="D511">
-        <v>145</v>
-      </c>
       <c r="E511" t="s">
         <v>7</v>
       </c>
       <c r="F511" t="s">
-        <v>253</v>
+        <v>529</v>
       </c>
       <c r="G511" t="s">
         <v>27</v>
@@ -15325,22 +15362,22 @@
     </row>
     <row r="512" spans="1:8" hidden="1">
       <c r="A512">
-        <v>2753</v>
+        <v>100175</v>
       </c>
       <c r="B512">
-        <v>649777</v>
+        <v>541000</v>
       </c>
       <c r="C512">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D512">
-        <v>274</v>
+        <v>17</v>
       </c>
       <c r="E512" t="s">
         <v>7</v>
       </c>
       <c r="F512" t="s">
-        <v>223</v>
+        <v>470</v>
       </c>
       <c r="G512" t="s">
         <v>27</v>
@@ -15375,7 +15412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="514" spans="1:8">
+    <row r="514" spans="1:8" hidden="1">
       <c r="A514">
         <v>13136</v>
       </c>
@@ -15403,22 +15440,22 @@
     </row>
     <row r="515" spans="1:8" hidden="1">
       <c r="A515">
-        <v>168934</v>
+        <v>84567</v>
       </c>
       <c r="B515">
-        <v>41295</v>
+        <v>84566</v>
       </c>
       <c r="C515">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D515">
-        <v>299</v>
+        <v>17</v>
       </c>
       <c r="E515" t="s">
         <v>7</v>
       </c>
       <c r="F515" t="s">
-        <v>219</v>
+        <v>537</v>
       </c>
       <c r="G515" t="s">
         <v>27</v>
@@ -15429,22 +15466,22 @@
     </row>
     <row r="516" spans="1:8" hidden="1">
       <c r="A516">
-        <v>278993</v>
+        <v>836</v>
       </c>
       <c r="B516">
-        <v>186807</v>
+        <v>171551</v>
       </c>
       <c r="C516">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D516">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E516" t="s">
         <v>7</v>
       </c>
       <c r="F516" t="s">
-        <v>420</v>
+        <v>442</v>
       </c>
       <c r="G516" t="s">
         <v>27</v>
@@ -15453,7 +15490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="517" spans="1:8">
+    <row r="517" spans="1:8" hidden="1">
       <c r="A517">
         <v>184870</v>
       </c>
@@ -15533,10 +15570,10 @@
     </row>
     <row r="520" spans="1:8" hidden="1">
       <c r="A520">
-        <v>32012</v>
+        <v>100132</v>
       </c>
       <c r="B520">
-        <v>224471</v>
+        <v>186803</v>
       </c>
       <c r="C520">
         <v>2</v>
@@ -15548,7 +15585,7 @@
         <v>7</v>
       </c>
       <c r="F520" t="s">
-        <v>480</v>
+        <v>528</v>
       </c>
       <c r="G520" t="s">
         <v>27</v>
@@ -15559,22 +15596,22 @@
     </row>
     <row r="521" spans="1:8" hidden="1">
       <c r="A521">
-        <v>191303</v>
+        <v>1279</v>
       </c>
       <c r="B521">
-        <v>128827</v>
+        <v>90964</v>
       </c>
       <c r="C521">
-        <v>103</v>
+        <v>2</v>
       </c>
       <c r="D521">
-        <v>881</v>
+        <v>17</v>
       </c>
       <c r="E521" t="s">
         <v>7</v>
       </c>
       <c r="F521" t="s">
-        <v>156</v>
+        <v>437</v>
       </c>
       <c r="G521" t="s">
         <v>27</v>
@@ -15611,22 +15648,22 @@
     </row>
     <row r="523" spans="1:8" hidden="1">
       <c r="A523">
-        <v>184869</v>
+        <v>32012</v>
       </c>
       <c r="B523">
-        <v>2049</v>
+        <v>224471</v>
       </c>
       <c r="C523">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D523">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="E523" t="s">
         <v>7</v>
       </c>
       <c r="F523" t="s">
-        <v>313</v>
+        <v>480</v>
       </c>
       <c r="G523" t="s">
         <v>27</v>
@@ -15635,7 +15672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="524" spans="1:8">
+    <row r="524" spans="1:8" hidden="1">
       <c r="A524">
         <v>573638</v>
       </c>
@@ -15691,12 +15728,152 @@
   <autoFilter ref="A1:H525">
     <filterColumn colId="6">
       <filters>
-        <filter val="species"/>
-        <filter val="species_group"/>
+        <filter val="phylum"/>
       </filters>
     </filterColumn>
-    <sortState ref="A3:H468">
+    <sortState ref="A12:H523">
       <sortCondition descending="1" ref="D1:D525"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>41435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>10045</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>547</v>
+      </c>
+      <c r="B4">
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>544</v>
+      </c>
+      <c r="B6">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B7">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>548</v>
+      </c>
+      <c r="B9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>546</v>
+      </c>
+      <c r="B11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B14">
+    <sortState ref="A2:B14">
+      <sortCondition descending="1" ref="B1:B14"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>